<commit_message>
Implementation of yr1 & testing
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="491" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="802" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="416">
   <si>
     <t>[h]</t>
   </si>
@@ -1252,6 +1252,9 @@
   </si>
   <si>
     <t>S100A4</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>erythrocytes</t>
@@ -1327,7 +1330,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1350,6 +1353,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1387,7 +1396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1552,11 +1561,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1569,20 +1590,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <sz val="10"/>
@@ -1681,7 +1689,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:AW42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C41:E41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2544,7 +2552,7 @@
   <dimension ref="A1:AA42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB42" activeCellId="0" sqref="A2:AW42"/>
+      <selection pane="topLeft" activeCell="AB42" activeCellId="1" sqref="C41:E41 AB42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6045,7 +6053,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="A2:AW42"/>
+      <selection pane="topLeft" activeCell="AW2" activeCellId="1" sqref="C41:E41 AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13372,7 +13380,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="A2:AW42"/>
+      <selection pane="topLeft" activeCell="AW2" activeCellId="1" sqref="C41:E41 AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -20640,7 +20648,7 @@
   <dimension ref="A1:AX42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:AW42"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C41:E41 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26931,10 +26939,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX42"/>
+  <dimension ref="1:42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW42" activeCellId="0" sqref="A2:AW42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW42" activeCellId="1" sqref="C41:E41 AW42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26944,6 +26952,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30" t="s">
         <v>313</v>
@@ -27086,6 +27095,981 @@
       <c r="AW1" s="30" t="s">
         <v>358</v>
       </c>
+      <c r="AX1" s="0"/>
+      <c r="AY1" s="0"/>
+      <c r="AZ1" s="0"/>
+      <c r="BA1" s="0"/>
+      <c r="BB1" s="0"/>
+      <c r="BC1" s="0"/>
+      <c r="BD1" s="0"/>
+      <c r="BE1" s="0"/>
+      <c r="BF1" s="0"/>
+      <c r="BG1" s="0"/>
+      <c r="BH1" s="0"/>
+      <c r="BI1" s="0"/>
+      <c r="BJ1" s="0"/>
+      <c r="BK1" s="0"/>
+      <c r="BL1" s="0"/>
+      <c r="BM1" s="0"/>
+      <c r="BN1" s="0"/>
+      <c r="BO1" s="0"/>
+      <c r="BP1" s="0"/>
+      <c r="BQ1" s="0"/>
+      <c r="BR1" s="0"/>
+      <c r="BS1" s="0"/>
+      <c r="BT1" s="0"/>
+      <c r="BU1" s="0"/>
+      <c r="BV1" s="0"/>
+      <c r="BW1" s="0"/>
+      <c r="BX1" s="0"/>
+      <c r="BY1" s="0"/>
+      <c r="BZ1" s="0"/>
+      <c r="CA1" s="0"/>
+      <c r="CB1" s="0"/>
+      <c r="CC1" s="0"/>
+      <c r="CD1" s="0"/>
+      <c r="CE1" s="0"/>
+      <c r="CF1" s="0"/>
+      <c r="CG1" s="0"/>
+      <c r="CH1" s="0"/>
+      <c r="CI1" s="0"/>
+      <c r="CJ1" s="0"/>
+      <c r="CK1" s="0"/>
+      <c r="CL1" s="0"/>
+      <c r="CM1" s="0"/>
+      <c r="CN1" s="0"/>
+      <c r="CO1" s="0"/>
+      <c r="CP1" s="0"/>
+      <c r="CQ1" s="0"/>
+      <c r="CR1" s="0"/>
+      <c r="CS1" s="0"/>
+      <c r="CT1" s="0"/>
+      <c r="CU1" s="0"/>
+      <c r="CV1" s="0"/>
+      <c r="CW1" s="0"/>
+      <c r="CX1" s="0"/>
+      <c r="CY1" s="0"/>
+      <c r="CZ1" s="0"/>
+      <c r="DA1" s="0"/>
+      <c r="DB1" s="0"/>
+      <c r="DC1" s="0"/>
+      <c r="DD1" s="0"/>
+      <c r="DE1" s="0"/>
+      <c r="DF1" s="0"/>
+      <c r="DG1" s="0"/>
+      <c r="DH1" s="0"/>
+      <c r="DI1" s="0"/>
+      <c r="DJ1" s="0"/>
+      <c r="DK1" s="0"/>
+      <c r="DL1" s="0"/>
+      <c r="DM1" s="0"/>
+      <c r="DN1" s="0"/>
+      <c r="DO1" s="0"/>
+      <c r="DP1" s="0"/>
+      <c r="DQ1" s="0"/>
+      <c r="DR1" s="0"/>
+      <c r="DS1" s="0"/>
+      <c r="DT1" s="0"/>
+      <c r="DU1" s="0"/>
+      <c r="DV1" s="0"/>
+      <c r="DW1" s="0"/>
+      <c r="DX1" s="0"/>
+      <c r="DY1" s="0"/>
+      <c r="DZ1" s="0"/>
+      <c r="EA1" s="0"/>
+      <c r="EB1" s="0"/>
+      <c r="EC1" s="0"/>
+      <c r="ED1" s="0"/>
+      <c r="EE1" s="0"/>
+      <c r="EF1" s="0"/>
+      <c r="EG1" s="0"/>
+      <c r="EH1" s="0"/>
+      <c r="EI1" s="0"/>
+      <c r="EJ1" s="0"/>
+      <c r="EK1" s="0"/>
+      <c r="EL1" s="0"/>
+      <c r="EM1" s="0"/>
+      <c r="EN1" s="0"/>
+      <c r="EO1" s="0"/>
+      <c r="EP1" s="0"/>
+      <c r="EQ1" s="0"/>
+      <c r="ER1" s="0"/>
+      <c r="ES1" s="0"/>
+      <c r="ET1" s="0"/>
+      <c r="EU1" s="0"/>
+      <c r="EV1" s="0"/>
+      <c r="EW1" s="0"/>
+      <c r="EX1" s="0"/>
+      <c r="EY1" s="0"/>
+      <c r="EZ1" s="0"/>
+      <c r="FA1" s="0"/>
+      <c r="FB1" s="0"/>
+      <c r="FC1" s="0"/>
+      <c r="FD1" s="0"/>
+      <c r="FE1" s="0"/>
+      <c r="FF1" s="0"/>
+      <c r="FG1" s="0"/>
+      <c r="FH1" s="0"/>
+      <c r="FI1" s="0"/>
+      <c r="FJ1" s="0"/>
+      <c r="FK1" s="0"/>
+      <c r="FL1" s="0"/>
+      <c r="FM1" s="0"/>
+      <c r="FN1" s="0"/>
+      <c r="FO1" s="0"/>
+      <c r="FP1" s="0"/>
+      <c r="FQ1" s="0"/>
+      <c r="FR1" s="0"/>
+      <c r="FS1" s="0"/>
+      <c r="FT1" s="0"/>
+      <c r="FU1" s="0"/>
+      <c r="FV1" s="0"/>
+      <c r="FW1" s="0"/>
+      <c r="FX1" s="0"/>
+      <c r="FY1" s="0"/>
+      <c r="FZ1" s="0"/>
+      <c r="GA1" s="0"/>
+      <c r="GB1" s="0"/>
+      <c r="GC1" s="0"/>
+      <c r="GD1" s="0"/>
+      <c r="GE1" s="0"/>
+      <c r="GF1" s="0"/>
+      <c r="GG1" s="0"/>
+      <c r="GH1" s="0"/>
+      <c r="GI1" s="0"/>
+      <c r="GJ1" s="0"/>
+      <c r="GK1" s="0"/>
+      <c r="GL1" s="0"/>
+      <c r="GM1" s="0"/>
+      <c r="GN1" s="0"/>
+      <c r="GO1" s="0"/>
+      <c r="GP1" s="0"/>
+      <c r="GQ1" s="0"/>
+      <c r="GR1" s="0"/>
+      <c r="GS1" s="0"/>
+      <c r="GT1" s="0"/>
+      <c r="GU1" s="0"/>
+      <c r="GV1" s="0"/>
+      <c r="GW1" s="0"/>
+      <c r="GX1" s="0"/>
+      <c r="GY1" s="0"/>
+      <c r="GZ1" s="0"/>
+      <c r="HA1" s="0"/>
+      <c r="HB1" s="0"/>
+      <c r="HC1" s="0"/>
+      <c r="HD1" s="0"/>
+      <c r="HE1" s="0"/>
+      <c r="HF1" s="0"/>
+      <c r="HG1" s="0"/>
+      <c r="HH1" s="0"/>
+      <c r="HI1" s="0"/>
+      <c r="HJ1" s="0"/>
+      <c r="HK1" s="0"/>
+      <c r="HL1" s="0"/>
+      <c r="HM1" s="0"/>
+      <c r="HN1" s="0"/>
+      <c r="HO1" s="0"/>
+      <c r="HP1" s="0"/>
+      <c r="HQ1" s="0"/>
+      <c r="HR1" s="0"/>
+      <c r="HS1" s="0"/>
+      <c r="HT1" s="0"/>
+      <c r="HU1" s="0"/>
+      <c r="HV1" s="0"/>
+      <c r="HW1" s="0"/>
+      <c r="HX1" s="0"/>
+      <c r="HY1" s="0"/>
+      <c r="HZ1" s="0"/>
+      <c r="IA1" s="0"/>
+      <c r="IB1" s="0"/>
+      <c r="IC1" s="0"/>
+      <c r="ID1" s="0"/>
+      <c r="IE1" s="0"/>
+      <c r="IF1" s="0"/>
+      <c r="IG1" s="0"/>
+      <c r="IH1" s="0"/>
+      <c r="II1" s="0"/>
+      <c r="IJ1" s="0"/>
+      <c r="IK1" s="0"/>
+      <c r="IL1" s="0"/>
+      <c r="IM1" s="0"/>
+      <c r="IN1" s="0"/>
+      <c r="IO1" s="0"/>
+      <c r="IP1" s="0"/>
+      <c r="IQ1" s="0"/>
+      <c r="IR1" s="0"/>
+      <c r="IS1" s="0"/>
+      <c r="IT1" s="0"/>
+      <c r="IU1" s="0"/>
+      <c r="IV1" s="0"/>
+      <c r="IW1" s="0"/>
+      <c r="IX1" s="0"/>
+      <c r="IY1" s="0"/>
+      <c r="IZ1" s="0"/>
+      <c r="JA1" s="0"/>
+      <c r="JB1" s="0"/>
+      <c r="JC1" s="0"/>
+      <c r="JD1" s="0"/>
+      <c r="JE1" s="0"/>
+      <c r="JF1" s="0"/>
+      <c r="JG1" s="0"/>
+      <c r="JH1" s="0"/>
+      <c r="JI1" s="0"/>
+      <c r="JJ1" s="0"/>
+      <c r="JK1" s="0"/>
+      <c r="JL1" s="0"/>
+      <c r="JM1" s="0"/>
+      <c r="JN1" s="0"/>
+      <c r="JO1" s="0"/>
+      <c r="JP1" s="0"/>
+      <c r="JQ1" s="0"/>
+      <c r="JR1" s="0"/>
+      <c r="JS1" s="0"/>
+      <c r="JT1" s="0"/>
+      <c r="JU1" s="0"/>
+      <c r="JV1" s="0"/>
+      <c r="JW1" s="0"/>
+      <c r="JX1" s="0"/>
+      <c r="JY1" s="0"/>
+      <c r="JZ1" s="0"/>
+      <c r="KA1" s="0"/>
+      <c r="KB1" s="0"/>
+      <c r="KC1" s="0"/>
+      <c r="KD1" s="0"/>
+      <c r="KE1" s="0"/>
+      <c r="KF1" s="0"/>
+      <c r="KG1" s="0"/>
+      <c r="KH1" s="0"/>
+      <c r="KI1" s="0"/>
+      <c r="KJ1" s="0"/>
+      <c r="KK1" s="0"/>
+      <c r="KL1" s="0"/>
+      <c r="KM1" s="0"/>
+      <c r="KN1" s="0"/>
+      <c r="KO1" s="0"/>
+      <c r="KP1" s="0"/>
+      <c r="KQ1" s="0"/>
+      <c r="KR1" s="0"/>
+      <c r="KS1" s="0"/>
+      <c r="KT1" s="0"/>
+      <c r="KU1" s="0"/>
+      <c r="KV1" s="0"/>
+      <c r="KW1" s="0"/>
+      <c r="KX1" s="0"/>
+      <c r="KY1" s="0"/>
+      <c r="KZ1" s="0"/>
+      <c r="LA1" s="0"/>
+      <c r="LB1" s="0"/>
+      <c r="LC1" s="0"/>
+      <c r="LD1" s="0"/>
+      <c r="LE1" s="0"/>
+      <c r="LF1" s="0"/>
+      <c r="LG1" s="0"/>
+      <c r="LH1" s="0"/>
+      <c r="LI1" s="0"/>
+      <c r="LJ1" s="0"/>
+      <c r="LK1" s="0"/>
+      <c r="LL1" s="0"/>
+      <c r="LM1" s="0"/>
+      <c r="LN1" s="0"/>
+      <c r="LO1" s="0"/>
+      <c r="LP1" s="0"/>
+      <c r="LQ1" s="0"/>
+      <c r="LR1" s="0"/>
+      <c r="LS1" s="0"/>
+      <c r="LT1" s="0"/>
+      <c r="LU1" s="0"/>
+      <c r="LV1" s="0"/>
+      <c r="LW1" s="0"/>
+      <c r="LX1" s="0"/>
+      <c r="LY1" s="0"/>
+      <c r="LZ1" s="0"/>
+      <c r="MA1" s="0"/>
+      <c r="MB1" s="0"/>
+      <c r="MC1" s="0"/>
+      <c r="MD1" s="0"/>
+      <c r="ME1" s="0"/>
+      <c r="MF1" s="0"/>
+      <c r="MG1" s="0"/>
+      <c r="MH1" s="0"/>
+      <c r="MI1" s="0"/>
+      <c r="MJ1" s="0"/>
+      <c r="MK1" s="0"/>
+      <c r="ML1" s="0"/>
+      <c r="MM1" s="0"/>
+      <c r="MN1" s="0"/>
+      <c r="MO1" s="0"/>
+      <c r="MP1" s="0"/>
+      <c r="MQ1" s="0"/>
+      <c r="MR1" s="0"/>
+      <c r="MS1" s="0"/>
+      <c r="MT1" s="0"/>
+      <c r="MU1" s="0"/>
+      <c r="MV1" s="0"/>
+      <c r="MW1" s="0"/>
+      <c r="MX1" s="0"/>
+      <c r="MY1" s="0"/>
+      <c r="MZ1" s="0"/>
+      <c r="NA1" s="0"/>
+      <c r="NB1" s="0"/>
+      <c r="NC1" s="0"/>
+      <c r="ND1" s="0"/>
+      <c r="NE1" s="0"/>
+      <c r="NF1" s="0"/>
+      <c r="NG1" s="0"/>
+      <c r="NH1" s="0"/>
+      <c r="NI1" s="0"/>
+      <c r="NJ1" s="0"/>
+      <c r="NK1" s="0"/>
+      <c r="NL1" s="0"/>
+      <c r="NM1" s="0"/>
+      <c r="NN1" s="0"/>
+      <c r="NO1" s="0"/>
+      <c r="NP1" s="0"/>
+      <c r="NQ1" s="0"/>
+      <c r="NR1" s="0"/>
+      <c r="NS1" s="0"/>
+      <c r="NT1" s="0"/>
+      <c r="NU1" s="0"/>
+      <c r="NV1" s="0"/>
+      <c r="NW1" s="0"/>
+      <c r="NX1" s="0"/>
+      <c r="NY1" s="0"/>
+      <c r="NZ1" s="0"/>
+      <c r="OA1" s="0"/>
+      <c r="OB1" s="0"/>
+      <c r="OC1" s="0"/>
+      <c r="OD1" s="0"/>
+      <c r="OE1" s="0"/>
+      <c r="OF1" s="0"/>
+      <c r="OG1" s="0"/>
+      <c r="OH1" s="0"/>
+      <c r="OI1" s="0"/>
+      <c r="OJ1" s="0"/>
+      <c r="OK1" s="0"/>
+      <c r="OL1" s="0"/>
+      <c r="OM1" s="0"/>
+      <c r="ON1" s="0"/>
+      <c r="OO1" s="0"/>
+      <c r="OP1" s="0"/>
+      <c r="OQ1" s="0"/>
+      <c r="OR1" s="0"/>
+      <c r="OS1" s="0"/>
+      <c r="OT1" s="0"/>
+      <c r="OU1" s="0"/>
+      <c r="OV1" s="0"/>
+      <c r="OW1" s="0"/>
+      <c r="OX1" s="0"/>
+      <c r="OY1" s="0"/>
+      <c r="OZ1" s="0"/>
+      <c r="PA1" s="0"/>
+      <c r="PB1" s="0"/>
+      <c r="PC1" s="0"/>
+      <c r="PD1" s="0"/>
+      <c r="PE1" s="0"/>
+      <c r="PF1" s="0"/>
+      <c r="PG1" s="0"/>
+      <c r="PH1" s="0"/>
+      <c r="PI1" s="0"/>
+      <c r="PJ1" s="0"/>
+      <c r="PK1" s="0"/>
+      <c r="PL1" s="0"/>
+      <c r="PM1" s="0"/>
+      <c r="PN1" s="0"/>
+      <c r="PO1" s="0"/>
+      <c r="PP1" s="0"/>
+      <c r="PQ1" s="0"/>
+      <c r="PR1" s="0"/>
+      <c r="PS1" s="0"/>
+      <c r="PT1" s="0"/>
+      <c r="PU1" s="0"/>
+      <c r="PV1" s="0"/>
+      <c r="PW1" s="0"/>
+      <c r="PX1" s="0"/>
+      <c r="PY1" s="0"/>
+      <c r="PZ1" s="0"/>
+      <c r="QA1" s="0"/>
+      <c r="QB1" s="0"/>
+      <c r="QC1" s="0"/>
+      <c r="QD1" s="0"/>
+      <c r="QE1" s="0"/>
+      <c r="QF1" s="0"/>
+      <c r="QG1" s="0"/>
+      <c r="QH1" s="0"/>
+      <c r="QI1" s="0"/>
+      <c r="QJ1" s="0"/>
+      <c r="QK1" s="0"/>
+      <c r="QL1" s="0"/>
+      <c r="QM1" s="0"/>
+      <c r="QN1" s="0"/>
+      <c r="QO1" s="0"/>
+      <c r="QP1" s="0"/>
+      <c r="QQ1" s="0"/>
+      <c r="QR1" s="0"/>
+      <c r="QS1" s="0"/>
+      <c r="QT1" s="0"/>
+      <c r="QU1" s="0"/>
+      <c r="QV1" s="0"/>
+      <c r="QW1" s="0"/>
+      <c r="QX1" s="0"/>
+      <c r="QY1" s="0"/>
+      <c r="QZ1" s="0"/>
+      <c r="RA1" s="0"/>
+      <c r="RB1" s="0"/>
+      <c r="RC1" s="0"/>
+      <c r="RD1" s="0"/>
+      <c r="RE1" s="0"/>
+      <c r="RF1" s="0"/>
+      <c r="RG1" s="0"/>
+      <c r="RH1" s="0"/>
+      <c r="RI1" s="0"/>
+      <c r="RJ1" s="0"/>
+      <c r="RK1" s="0"/>
+      <c r="RL1" s="0"/>
+      <c r="RM1" s="0"/>
+      <c r="RN1" s="0"/>
+      <c r="RO1" s="0"/>
+      <c r="RP1" s="0"/>
+      <c r="RQ1" s="0"/>
+      <c r="RR1" s="0"/>
+      <c r="RS1" s="0"/>
+      <c r="RT1" s="0"/>
+      <c r="RU1" s="0"/>
+      <c r="RV1" s="0"/>
+      <c r="RW1" s="0"/>
+      <c r="RX1" s="0"/>
+      <c r="RY1" s="0"/>
+      <c r="RZ1" s="0"/>
+      <c r="SA1" s="0"/>
+      <c r="SB1" s="0"/>
+      <c r="SC1" s="0"/>
+      <c r="SD1" s="0"/>
+      <c r="SE1" s="0"/>
+      <c r="SF1" s="0"/>
+      <c r="SG1" s="0"/>
+      <c r="SH1" s="0"/>
+      <c r="SI1" s="0"/>
+      <c r="SJ1" s="0"/>
+      <c r="SK1" s="0"/>
+      <c r="SL1" s="0"/>
+      <c r="SM1" s="0"/>
+      <c r="SN1" s="0"/>
+      <c r="SO1" s="0"/>
+      <c r="SP1" s="0"/>
+      <c r="SQ1" s="0"/>
+      <c r="SR1" s="0"/>
+      <c r="SS1" s="0"/>
+      <c r="ST1" s="0"/>
+      <c r="SU1" s="0"/>
+      <c r="SV1" s="0"/>
+      <c r="SW1" s="0"/>
+      <c r="SX1" s="0"/>
+      <c r="SY1" s="0"/>
+      <c r="SZ1" s="0"/>
+      <c r="TA1" s="0"/>
+      <c r="TB1" s="0"/>
+      <c r="TC1" s="0"/>
+      <c r="TD1" s="0"/>
+      <c r="TE1" s="0"/>
+      <c r="TF1" s="0"/>
+      <c r="TG1" s="0"/>
+      <c r="TH1" s="0"/>
+      <c r="TI1" s="0"/>
+      <c r="TJ1" s="0"/>
+      <c r="TK1" s="0"/>
+      <c r="TL1" s="0"/>
+      <c r="TM1" s="0"/>
+      <c r="TN1" s="0"/>
+      <c r="TO1" s="0"/>
+      <c r="TP1" s="0"/>
+      <c r="TQ1" s="0"/>
+      <c r="TR1" s="0"/>
+      <c r="TS1" s="0"/>
+      <c r="TT1" s="0"/>
+      <c r="TU1" s="0"/>
+      <c r="TV1" s="0"/>
+      <c r="TW1" s="0"/>
+      <c r="TX1" s="0"/>
+      <c r="TY1" s="0"/>
+      <c r="TZ1" s="0"/>
+      <c r="UA1" s="0"/>
+      <c r="UB1" s="0"/>
+      <c r="UC1" s="0"/>
+      <c r="UD1" s="0"/>
+      <c r="UE1" s="0"/>
+      <c r="UF1" s="0"/>
+      <c r="UG1" s="0"/>
+      <c r="UH1" s="0"/>
+      <c r="UI1" s="0"/>
+      <c r="UJ1" s="0"/>
+      <c r="UK1" s="0"/>
+      <c r="UL1" s="0"/>
+      <c r="UM1" s="0"/>
+      <c r="UN1" s="0"/>
+      <c r="UO1" s="0"/>
+      <c r="UP1" s="0"/>
+      <c r="UQ1" s="0"/>
+      <c r="UR1" s="0"/>
+      <c r="US1" s="0"/>
+      <c r="UT1" s="0"/>
+      <c r="UU1" s="0"/>
+      <c r="UV1" s="0"/>
+      <c r="UW1" s="0"/>
+      <c r="UX1" s="0"/>
+      <c r="UY1" s="0"/>
+      <c r="UZ1" s="0"/>
+      <c r="VA1" s="0"/>
+      <c r="VB1" s="0"/>
+      <c r="VC1" s="0"/>
+      <c r="VD1" s="0"/>
+      <c r="VE1" s="0"/>
+      <c r="VF1" s="0"/>
+      <c r="VG1" s="0"/>
+      <c r="VH1" s="0"/>
+      <c r="VI1" s="0"/>
+      <c r="VJ1" s="0"/>
+      <c r="VK1" s="0"/>
+      <c r="VL1" s="0"/>
+      <c r="VM1" s="0"/>
+      <c r="VN1" s="0"/>
+      <c r="VO1" s="0"/>
+      <c r="VP1" s="0"/>
+      <c r="VQ1" s="0"/>
+      <c r="VR1" s="0"/>
+      <c r="VS1" s="0"/>
+      <c r="VT1" s="0"/>
+      <c r="VU1" s="0"/>
+      <c r="VV1" s="0"/>
+      <c r="VW1" s="0"/>
+      <c r="VX1" s="0"/>
+      <c r="VY1" s="0"/>
+      <c r="VZ1" s="0"/>
+      <c r="WA1" s="0"/>
+      <c r="WB1" s="0"/>
+      <c r="WC1" s="0"/>
+      <c r="WD1" s="0"/>
+      <c r="WE1" s="0"/>
+      <c r="WF1" s="0"/>
+      <c r="WG1" s="0"/>
+      <c r="WH1" s="0"/>
+      <c r="WI1" s="0"/>
+      <c r="WJ1" s="0"/>
+      <c r="WK1" s="0"/>
+      <c r="WL1" s="0"/>
+      <c r="WM1" s="0"/>
+      <c r="WN1" s="0"/>
+      <c r="WO1" s="0"/>
+      <c r="WP1" s="0"/>
+      <c r="WQ1" s="0"/>
+      <c r="WR1" s="0"/>
+      <c r="WS1" s="0"/>
+      <c r="WT1" s="0"/>
+      <c r="WU1" s="0"/>
+      <c r="WV1" s="0"/>
+      <c r="WW1" s="0"/>
+      <c r="WX1" s="0"/>
+      <c r="WY1" s="0"/>
+      <c r="WZ1" s="0"/>
+      <c r="XA1" s="0"/>
+      <c r="XB1" s="0"/>
+      <c r="XC1" s="0"/>
+      <c r="XD1" s="0"/>
+      <c r="XE1" s="0"/>
+      <c r="XF1" s="0"/>
+      <c r="XG1" s="0"/>
+      <c r="XH1" s="0"/>
+      <c r="XI1" s="0"/>
+      <c r="XJ1" s="0"/>
+      <c r="XK1" s="0"/>
+      <c r="XL1" s="0"/>
+      <c r="XM1" s="0"/>
+      <c r="XN1" s="0"/>
+      <c r="XO1" s="0"/>
+      <c r="XP1" s="0"/>
+      <c r="XQ1" s="0"/>
+      <c r="XR1" s="0"/>
+      <c r="XS1" s="0"/>
+      <c r="XT1" s="0"/>
+      <c r="XU1" s="0"/>
+      <c r="XV1" s="0"/>
+      <c r="XW1" s="0"/>
+      <c r="XX1" s="0"/>
+      <c r="XY1" s="0"/>
+      <c r="XZ1" s="0"/>
+      <c r="YA1" s="0"/>
+      <c r="YB1" s="0"/>
+      <c r="YC1" s="0"/>
+      <c r="YD1" s="0"/>
+      <c r="YE1" s="0"/>
+      <c r="YF1" s="0"/>
+      <c r="YG1" s="0"/>
+      <c r="YH1" s="0"/>
+      <c r="YI1" s="0"/>
+      <c r="YJ1" s="0"/>
+      <c r="YK1" s="0"/>
+      <c r="YL1" s="0"/>
+      <c r="YM1" s="0"/>
+      <c r="YN1" s="0"/>
+      <c r="YO1" s="0"/>
+      <c r="YP1" s="0"/>
+      <c r="YQ1" s="0"/>
+      <c r="YR1" s="0"/>
+      <c r="YS1" s="0"/>
+      <c r="YT1" s="0"/>
+      <c r="YU1" s="0"/>
+      <c r="YV1" s="0"/>
+      <c r="YW1" s="0"/>
+      <c r="YX1" s="0"/>
+      <c r="YY1" s="0"/>
+      <c r="YZ1" s="0"/>
+      <c r="ZA1" s="0"/>
+      <c r="ZB1" s="0"/>
+      <c r="ZC1" s="0"/>
+      <c r="ZD1" s="0"/>
+      <c r="ZE1" s="0"/>
+      <c r="ZF1" s="0"/>
+      <c r="ZG1" s="0"/>
+      <c r="ZH1" s="0"/>
+      <c r="ZI1" s="0"/>
+      <c r="ZJ1" s="0"/>
+      <c r="ZK1" s="0"/>
+      <c r="ZL1" s="0"/>
+      <c r="ZM1" s="0"/>
+      <c r="ZN1" s="0"/>
+      <c r="ZO1" s="0"/>
+      <c r="ZP1" s="0"/>
+      <c r="ZQ1" s="0"/>
+      <c r="ZR1" s="0"/>
+      <c r="ZS1" s="0"/>
+      <c r="ZT1" s="0"/>
+      <c r="ZU1" s="0"/>
+      <c r="ZV1" s="0"/>
+      <c r="ZW1" s="0"/>
+      <c r="ZX1" s="0"/>
+      <c r="ZY1" s="0"/>
+      <c r="ZZ1" s="0"/>
+      <c r="AAA1" s="0"/>
+      <c r="AAB1" s="0"/>
+      <c r="AAC1" s="0"/>
+      <c r="AAD1" s="0"/>
+      <c r="AAE1" s="0"/>
+      <c r="AAF1" s="0"/>
+      <c r="AAG1" s="0"/>
+      <c r="AAH1" s="0"/>
+      <c r="AAI1" s="0"/>
+      <c r="AAJ1" s="0"/>
+      <c r="AAK1" s="0"/>
+      <c r="AAL1" s="0"/>
+      <c r="AAM1" s="0"/>
+      <c r="AAN1" s="0"/>
+      <c r="AAO1" s="0"/>
+      <c r="AAP1" s="0"/>
+      <c r="AAQ1" s="0"/>
+      <c r="AAR1" s="0"/>
+      <c r="AAS1" s="0"/>
+      <c r="AAT1" s="0"/>
+      <c r="AAU1" s="0"/>
+      <c r="AAV1" s="0"/>
+      <c r="AAW1" s="0"/>
+      <c r="AAX1" s="0"/>
+      <c r="AAY1" s="0"/>
+      <c r="AAZ1" s="0"/>
+      <c r="ABA1" s="0"/>
+      <c r="ABB1" s="0"/>
+      <c r="ABC1" s="0"/>
+      <c r="ABD1" s="0"/>
+      <c r="ABE1" s="0"/>
+      <c r="ABF1" s="0"/>
+      <c r="ABG1" s="0"/>
+      <c r="ABH1" s="0"/>
+      <c r="ABI1" s="0"/>
+      <c r="ABJ1" s="0"/>
+      <c r="ABK1" s="0"/>
+      <c r="ABL1" s="0"/>
+      <c r="ABM1" s="0"/>
+      <c r="ABN1" s="0"/>
+      <c r="ABO1" s="0"/>
+      <c r="ABP1" s="0"/>
+      <c r="ABQ1" s="0"/>
+      <c r="ABR1" s="0"/>
+      <c r="ABS1" s="0"/>
+      <c r="ABT1" s="0"/>
+      <c r="ABU1" s="0"/>
+      <c r="ABV1" s="0"/>
+      <c r="ABW1" s="0"/>
+      <c r="ABX1" s="0"/>
+      <c r="ABY1" s="0"/>
+      <c r="ABZ1" s="0"/>
+      <c r="ACA1" s="0"/>
+      <c r="ACB1" s="0"/>
+      <c r="ACC1" s="0"/>
+      <c r="ACD1" s="0"/>
+      <c r="ACE1" s="0"/>
+      <c r="ACF1" s="0"/>
+      <c r="ACG1" s="0"/>
+      <c r="ACH1" s="0"/>
+      <c r="ACI1" s="0"/>
+      <c r="ACJ1" s="0"/>
+      <c r="ACK1" s="0"/>
+      <c r="ACL1" s="0"/>
+      <c r="ACM1" s="0"/>
+      <c r="ACN1" s="0"/>
+      <c r="ACO1" s="0"/>
+      <c r="ACP1" s="0"/>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
@@ -33271,10 +34255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="A2:AW42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -33321,9 +34305,15 @@
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="C3" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="n">
@@ -33332,75 +34322,117 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="C4" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="40" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
+      <c r="C5" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="41" t="n">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="C6" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="41" t="n">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="C7" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="41" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
+      <c r="C8" s="41" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="41" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="C9" s="41" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="41" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="C10" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="41" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="40" t="n">
@@ -33409,9 +34441,16 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="C11" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="F11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="40" t="n">
@@ -33420,42 +34459,66 @@
       <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="C12" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="40" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="C13" s="41" t="n">
+        <v>15</v>
+      </c>
+      <c r="D13" s="41" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" s="41" t="n">
+        <v>15</v>
+      </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="C14" s="41" t="n">
+        <v>14</v>
+      </c>
+      <c r="D14" s="41" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" s="41" t="n">
+        <v>19</v>
+      </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="40" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="C15" s="41" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" s="41" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="n">
@@ -33464,9 +34527,15 @@
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="C16" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="n">
@@ -33475,31 +34544,49 @@
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="C17" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="C18" s="41" t="n">
+        <v>23</v>
+      </c>
+      <c r="D18" s="41" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" s="41" t="n">
+        <v>23</v>
+      </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="C19" s="41" t="n">
+        <v>34</v>
+      </c>
+      <c r="D19" s="41" t="n">
+        <v>16</v>
+      </c>
+      <c r="E19" s="41" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="n">
@@ -33508,20 +34595,32 @@
       <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="C20" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="C21" s="41" t="n">
+        <v>17</v>
+      </c>
+      <c r="D21" s="41" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" s="41" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="n">
@@ -33530,31 +34629,49 @@
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="C22" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="C23" s="41" t="n">
+        <v>45</v>
+      </c>
+      <c r="D23" s="41" t="n">
+        <v>19</v>
+      </c>
+      <c r="E23" s="41" t="n">
+        <v>25</v>
+      </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="41" t="n">
+        <v>69</v>
+      </c>
+      <c r="D24" s="41" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" s="41" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="n">
@@ -33563,20 +34680,32 @@
       <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="C25" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="C26" s="41" t="n">
+        <v>18</v>
+      </c>
+      <c r="D26" s="41" t="n">
+        <v>14</v>
+      </c>
+      <c r="E26" s="41" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="n">
@@ -33585,42 +34714,67 @@
       <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="C27" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="F27" s="42"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="C28" s="41" t="n">
+        <v>51</v>
+      </c>
+      <c r="D28" s="41" t="n">
+        <v>36</v>
+      </c>
+      <c r="E28" s="41" t="n">
+        <v>54</v>
+      </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="n">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="C29" s="41" t="n">
+        <v>76</v>
+      </c>
+      <c r="D29" s="41" t="n">
+        <v>41</v>
+      </c>
+      <c r="E29" s="41" t="n">
+        <v>61</v>
+      </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="n">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="C30" s="41" t="n">
+        <v>32</v>
+      </c>
+      <c r="D30" s="41" t="n">
+        <v>42</v>
+      </c>
+      <c r="E30" s="41" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="n">
@@ -33629,9 +34783,16 @@
       <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
+      <c r="C31" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="F31" s="42"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="40" t="n">
@@ -33640,9 +34801,16 @@
       <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
+      <c r="C32" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="F32" s="42"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="40" t="n">
@@ -33651,31 +34819,49 @@
       <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
+      <c r="C33" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="n">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
+      <c r="C34" s="41" t="n">
+        <v>89</v>
+      </c>
+      <c r="D34" s="41" t="n">
+        <v>66</v>
+      </c>
+      <c r="E34" s="41" t="n">
+        <v>44</v>
+      </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="40" t="n">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
+      <c r="C35" s="41" t="n">
+        <v>83</v>
+      </c>
+      <c r="D35" s="41" t="n">
+        <v>53</v>
+      </c>
+      <c r="E35" s="41" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="40" t="n">
@@ -33684,31 +34870,49 @@
       <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
+      <c r="C36" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="40" t="n">
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+      <c r="C37" s="41" t="n">
+        <v>45</v>
+      </c>
+      <c r="D37" s="41" t="n">
+        <v>41</v>
+      </c>
+      <c r="E37" s="41" t="n">
+        <v>55</v>
+      </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="40" t="n">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
+      <c r="C38" s="41" t="n">
+        <v>112</v>
+      </c>
+      <c r="D38" s="41" t="n">
+        <v>79</v>
+      </c>
+      <c r="E38" s="41" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="40" t="n">
@@ -33717,20 +34921,32 @@
       <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
+      <c r="C39" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>410</v>
+      </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="40" t="n">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
+      <c r="C40" s="41" t="n">
+        <v>123</v>
+      </c>
+      <c r="D40" s="41" t="n">
+        <v>85</v>
+      </c>
+      <c r="E40" s="41" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="40" t="n">
@@ -33739,20 +34955,33 @@
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
+      <c r="C41" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="F41" s="42"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="40" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
+      <c r="C42" s="41" t="n">
+        <v>87</v>
+      </c>
+      <c r="D42" s="41" t="n">
+        <v>87</v>
+      </c>
+      <c r="E42" s="41" t="n">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -33773,14 +35002,14 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="A2:AW42"/>
+      <selection pane="topLeft" activeCell="J33" activeCellId="1" sqref="C41:E41 J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="42" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="42" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="42" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="44" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33810,19 +35039,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33832,11 +35061,11 @@
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="n">
@@ -33845,11 +35074,11 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="40" t="n">
@@ -33858,11 +35087,11 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="n">
@@ -33871,11 +35100,11 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40" t="n">
@@ -33884,11 +35113,11 @@
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="n">
@@ -33897,11 +35126,11 @@
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="n">
@@ -33910,11 +35139,11 @@
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="n">
@@ -33923,11 +35152,11 @@
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="40" t="n">
@@ -33936,11 +35165,11 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="40" t="n">
@@ -33949,11 +35178,11 @@
       <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="40" t="n">
@@ -33962,11 +35191,11 @@
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40" t="n">
@@ -33975,11 +35204,11 @@
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="40" t="n">
@@ -33988,11 +35217,11 @@
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="n">
@@ -34001,11 +35230,11 @@
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="n">
@@ -34014,11 +35243,11 @@
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="n">
@@ -34027,11 +35256,11 @@
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="n">
@@ -34040,11 +35269,11 @@
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="n">
@@ -34053,11 +35282,11 @@
       <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="n">
@@ -34066,11 +35295,11 @@
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="n">
@@ -34079,11 +35308,11 @@
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="n">
@@ -34092,11 +35321,11 @@
       <c r="B23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="n">
@@ -34105,11 +35334,11 @@
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="n">
@@ -34118,11 +35347,11 @@
       <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="n">
@@ -34131,11 +35360,11 @@
       <c r="B26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="n">
@@ -34144,11 +35373,11 @@
       <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="n">
@@ -34157,11 +35386,11 @@
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="n">
@@ -34170,11 +35399,11 @@
       <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="n">
@@ -34183,11 +35412,11 @@
       <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="n">
@@ -34196,11 +35425,11 @@
       <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="40" t="n">
@@ -34209,11 +35438,11 @@
       <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="40" t="n">
@@ -34222,11 +35451,11 @@
       <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="n">
@@ -34235,11 +35464,11 @@
       <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="40" t="n">
@@ -34248,11 +35477,11 @@
       <c r="B35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="40" t="n">
@@ -34261,11 +35490,11 @@
       <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="40" t="n">
@@ -34274,11 +35503,11 @@
       <c r="B37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="40" t="n">
@@ -34287,11 +35516,11 @@
       <c r="B38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="40" t="n">
@@ -34300,11 +35529,11 @@
       <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="40" t="n">
@@ -34313,11 +35542,11 @@
       <c r="B40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="40" t="n">
@@ -34326,11 +35555,11 @@
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="40" t="n">
@@ -34339,11 +35568,11 @@
       <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>